<commit_message>
Fixed up error with RemoveAllKilledPartyMembers(). Violent Weather now working
</commit_message>
<xml_diff>
--- a/Config/Events.xlsx
+++ b/Config/Events.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\Documents\Visual Studio 2022\Projects\2024-04-16-Barbarian Prince\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\Documents\Visual Studio 2022\Projects\BarbarianPrince\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9DF9B6-AF8B-41CA-A57F-B509773B349F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C9751601-DD99-4CFF-BC4F-AE7C9C37190C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="26715" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -33517,181 +33517,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve"> &lt;Bold&gt;e105a Violent Weather&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Your party is blown out of control by gigantic winds. Roll one die for the direction you are blown instead of making your normal travel move:
-&lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;   1-N, 2-NE, 3-SE, 4-S, 5-SW, 6-NW
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die again and halve the number rounded up for the number of hexes your party is blown.
-&lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DieRoll1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You crash into the final hex. Your flying mount is killed and you roll one die for wounds suffered: 
-&lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DieRoll2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;All other members of your party are blown off course and lost to you.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                              &lt;InlineUIContainer&gt;&lt;Image Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>AirViolentWeather</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ViolentWeather</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>&lt;Bold&gt;e079b Heavy Rains Continues With Mounts&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;If you travel at all &lt;InlineUIContainer&gt;&lt;Button Content='r204' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, any characters who have not caught cold must risk it. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;If you ride your mounts, they may catch pneumonia. Roll one die for each. If they roll a 5 plus, they fall sick and die. You can &lt;InlineUIContainer&gt;&lt;Button Content='Dismount' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; and walk with the animals and avoid them getting sick. 
@@ -33718,6 +33543,181 @@
         <scheme val="minor"/>
       </rPr>
       <t>.gif' Height='220'  Width='440'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> &lt;Bold&gt;e105a Violent Weather&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Your party is blown out of control by gigantic winds. Roll one die for the direction you are blown instead of making your normal travel move: 
+&lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;   1-N, 2-NE, 3-SE, 4-S, 5-SW, 6-NW
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die again and halve the number rounded up for the number of hexes your party is blown: 
+&lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DieRoll1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You crash into the final hex. Your flying mount is killed and you roll one die for wounds suffered: 
+&lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dieRoll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DieRoll2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;All other members of your party are blown off course and lost to you.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                     &lt;InlineUIContainer&gt;&lt;Image Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AirViolentWeather</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ViolentWeather</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Height='200' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
     </r>
   </si>
 </sst>
@@ -34191,8 +34191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:XFD559"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A554" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B557" sqref="B557"/>
+    <sheetView tabSelected="1" topLeftCell="A280" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B282" sqref="B282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52420,7 +52420,7 @@
         <v>978</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -52836,7 +52836,7 @@
         <v>242</v>
       </c>
       <c r="B282" s="4" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="120" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix issue with violent weather. Now all working. Also there was a problem with MovePathAnimate()
</commit_message>
<xml_diff>
--- a/Config/Events.xlsx
+++ b/Config/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\Documents\Visual Studio 2022\Projects\BarbarianPrince\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C9751601-DD99-4CFF-BC4F-AE7C9C37190C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD62655C-CB13-4E72-8E7B-31F5BCC6DBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -34192,7 +34192,7 @@
   <dimension ref="A1:XFD559"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A280" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B282" sqref="B282"/>
+      <selection activeCell="B281" sqref="B281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finished E109 Wild Pegasus event. Additionally, removed pegasus that are starving if they cannot fly
</commit_message>
<xml_diff>
--- a/Config/Events.xlsx
+++ b/Config/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\Documents\Visual Studio 2022\Projects\BarbarianPrince2\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ADDB2AA-D3F1-4864-8625-854A9F175FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFCD6986-FECC-4EA0-89AE-EF0866025916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -33228,96 +33228,6 @@
   </si>
   <si>
     <r>
-      <t>&lt;Bold&gt;e109 Wild Pegasus&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You encounter a wild Pegasus. Each character in your party is allowed one attempt to capture it.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die: &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DieRoll</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='21'  Width='21' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If the result is 5 plus, the character captures the Pegasus. You may add it as a winged mount to your party.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                 &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Pegasus</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>EncounterEnd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>&lt;Bold&gt;e106 Heavy Overcast&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Thick, black clouds obscure your vision. You realize you are becoming lost. Roll one die for directions: 
 &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
@@ -33762,6 +33672,56 @@
         <scheme val="minor"/>
       </rPr>
       <t>.gif' Height='188' Width='250'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;e109 Wild Pegasus&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You encounter a wild Pegasus. Each character in your party is allowed one attempt to capture it.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die. If the result is 5 plus, the character captures the Pegasus. You may add it as a winged mount to your party.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Click image to continue.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                 &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pegasus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PegasusCapture</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
     </r>
   </si>
 </sst>
@@ -33895,7 +33855,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -33909,13 +33869,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -33937,9 +33893,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -33977,7 +33933,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -34083,7 +34039,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -34225,7 +34181,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -52411,35 +52367,35 @@
         <v>787</v>
       </c>
     </row>
-    <row r="224" spans="1:2" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A224" s="5" t="s">
+    <row r="224" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A224" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B224" s="6" t="s">
+      <c r="B224" s="5" t="s">
         <v>865</v>
       </c>
     </row>
-    <row r="225" spans="1:2" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A225" s="5" t="s">
+    <row r="225" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A225" s="2" t="s">
         <v>788</v>
       </c>
-      <c r="B225" s="6" t="s">
+      <c r="B225" s="5" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="226" spans="1:2" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A226" s="5" t="s">
+    <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A226" s="2" t="s">
         <v>789</v>
       </c>
-      <c r="B226" s="6" t="s">
+      <c r="B226" s="5" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="227" spans="1:2" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A227" s="5" t="s">
+    <row r="227" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A227" s="2" t="s">
         <v>792</v>
       </c>
-      <c r="B227" s="6" t="s">
+      <c r="B227" s="5" t="s">
         <v>979</v>
       </c>
     </row>
@@ -52464,7 +52420,7 @@
         <v>977</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -52872,7 +52828,7 @@
         <v>144</v>
       </c>
       <c r="B281" s="4" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -52880,7 +52836,7 @@
         <v>242</v>
       </c>
       <c r="B282" s="4" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -52888,7 +52844,7 @@
         <v>145</v>
       </c>
       <c r="B283" s="4" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -52896,7 +52852,7 @@
         <v>146</v>
       </c>
       <c r="B284" s="4" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -52912,7 +52868,7 @@
         <v>148</v>
       </c>
       <c r="B286" s="4" t="s">
-        <v>1112</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -53784,11 +53740,11 @@
         <v>684</v>
       </c>
     </row>
-    <row r="394" spans="1:2" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A394" s="5" t="s">
+    <row r="394" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A394" s="2" t="s">
         <v>679</v>
       </c>
-      <c r="B394" s="6" t="s">
+      <c r="B394" s="5" t="s">
         <v>685</v>
       </c>
     </row>
@@ -53969,7 +53925,7 @@
       </c>
     </row>
     <row r="417" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A417" s="8" t="s">
+      <c r="A417" s="6" t="s">
         <v>220</v>
       </c>
       <c r="B417" s="4" t="s">

</xml_diff>